<commit_message>
Started admin assigning lawyer user story
</commit_message>
<xml_diff>
--- a/Sprint3_Backlog.xlsx
+++ b/Sprint3_Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="41">
   <si>
     <t>User story</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Comments  Delete JEST Tests</t>
+  </si>
+  <si>
+    <t>As a lawyer I can fill a form</t>
   </si>
 </sst>
 </file>
@@ -494,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,7 +599,7 @@
         <v>29</v>
       </c>
       <c r="C5">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -836,7 +839,7 @@
         <v>17</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
@@ -1006,6 +1009,26 @@
       </c>
       <c r="F25" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Admin assigns, lawyer fills form, 2 usert [Cstories done
</commit_message>
<xml_diff>
--- a/Sprint3_Backlog.xlsx
+++ b/Sprint3_Backlog.xlsx
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Sprint 3 backlog updated
</commit_message>
<xml_diff>
--- a/Sprint3_Backlog.xlsx
+++ b/Sprint3_Backlog.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\6th Semester\CSEN 603 - Software Engineering\Sumerge Project\El-Lathaleeth\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="16275" windowHeight="9270"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="40">
   <si>
     <t>User story</t>
   </si>
@@ -34,9 +39,6 @@
   </si>
   <si>
     <t>Reviewers 1</t>
-  </si>
-  <si>
-    <t>Nadeen Amr</t>
   </si>
   <si>
     <t>Peter</t>
@@ -253,7 +255,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -288,7 +290,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -500,7 +502,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,19 +538,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -556,19 +558,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -576,19 +578,19 @@
         <v>3.1</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -596,19 +598,19 @@
         <v>3.2</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -616,19 +618,19 @@
         <v>3.3</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -636,19 +638,19 @@
         <v>3.4</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -656,19 +658,19 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -676,19 +678,19 @@
         <v>4.2</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -696,19 +698,19 @@
         <v>4.3</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -716,19 +718,19 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -736,19 +738,19 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -756,19 +758,19 @@
         <v>5.2</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -776,19 +778,19 @@
         <v>5.3</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -796,19 +798,19 @@
         <v>5.4</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -816,19 +818,19 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -836,19 +838,19 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -856,19 +858,19 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -876,19 +878,19 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -896,19 +898,19 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -916,19 +918,19 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -936,19 +938,19 @@
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
       <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
         <v>10</v>
       </c>
-      <c r="E22" t="s">
-        <v>11</v>
-      </c>
       <c r="F22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -956,19 +958,19 @@
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23">
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -976,19 +978,19 @@
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
       <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
         <v>9</v>
       </c>
-      <c r="E24" t="s">
-        <v>10</v>
-      </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -996,19 +998,19 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1016,19 +1018,19 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26">
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>